<commit_message>
Building a histogram of resistance to the number of isolates
</commit_message>
<xml_diff>
--- a/AMR_datasets/2014/K-pneumoniae/k-pneumoniae-resistance-combinations-2014.xlsx
+++ b/AMR_datasets/2014/K-pneumoniae/k-pneumoniae-resistance-combinations-2014.xlsx
@@ -112,7 +112,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,12 +123,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -232,71 +226,71 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">

</xml_diff>